<commit_message>
Updated README, filenames and added index to the pdf test suite
</commit_message>
<xml_diff>
--- a/ChargeX-ITP Navigator Builder/Interoperability Test Plan Version 2.xlsx
+++ b/ChargeX-ITP Navigator Builder/Interoperability Test Plan Version 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvartak\Box\ChargeX Root Folder\INTERNAL FOLDERS ONLY\Testing Task Force - Internal Folder\2 - Interop Test Plans\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvartak\Box\ChargeX Root Folder\INTERNAL FOLDERS ONLY\Testing Task Force - Internal Folder\2 - Interop Test Plans\6 - Github Upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5CCDC4-FEF7-484D-9ACC-C08C163BAF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92577864-EC17-4C45-8E5C-DB997B7515B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{51FF454D-C914-4A81-98D8-5224C5AD8D92}"/>
+    <workbookView xWindow="-28920" yWindow="-3810" windowWidth="29040" windowHeight="15720" xr2:uid="{51FF454D-C914-4A81-98D8-5224C5AD8D92}"/>
   </bookViews>
   <sheets>
     <sheet name="Detailed Test Cases" sheetId="4" r:id="rId1"/>
@@ -25746,7 +25746,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -25769,12 +25769,6 @@
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.499984740745262"/>
         <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -26682,11 +26676,65 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -26694,8 +26742,53 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -26723,105 +26816,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -26859,40 +26853,40 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -27268,11 +27262,11 @@
   </sheetPr>
   <dimension ref="A1:Q121"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A20" sqref="A20:XFD20"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -34130,8 +34124,8 @@
     <row r="2" spans="1:78" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="17"/>
       <c r="B2" s="18"/>
-      <c r="C2" s="110"/>
-      <c r="D2" s="110"/>
+      <c r="C2" s="147"/>
+      <c r="D2" s="147"/>
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
@@ -34141,28 +34135,28 @@
     </row>
     <row r="3" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="20"/>
-      <c r="B3" s="118" t="s">
+      <c r="B3" s="151" t="s">
         <v>344</v>
       </c>
-      <c r="C3" s="119"/>
-      <c r="D3" s="119"/>
-      <c r="E3" s="119"/>
-      <c r="F3" s="119"/>
-      <c r="G3" s="119"/>
-      <c r="H3" s="119"/>
-      <c r="I3" s="120"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
+      <c r="E3" s="152"/>
+      <c r="F3" s="152"/>
+      <c r="G3" s="152"/>
+      <c r="H3" s="152"/>
+      <c r="I3" s="153"/>
       <c r="J3" s="21"/>
     </row>
     <row r="4" spans="1:78" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="20"/>
-      <c r="B4" s="121"/>
-      <c r="C4" s="122"/>
-      <c r="D4" s="122"/>
-      <c r="E4" s="122"/>
-      <c r="F4" s="122"/>
-      <c r="G4" s="122"/>
-      <c r="H4" s="122"/>
-      <c r="I4" s="123"/>
+      <c r="B4" s="154"/>
+      <c r="C4" s="155"/>
+      <c r="D4" s="155"/>
+      <c r="E4" s="155"/>
+      <c r="F4" s="155"/>
+      <c r="G4" s="155"/>
+      <c r="H4" s="155"/>
+      <c r="I4" s="156"/>
       <c r="J4" s="21"/>
     </row>
     <row r="5" spans="1:78" x14ac:dyDescent="0.55000000000000004">
@@ -34170,13 +34164,13 @@
       <c r="B5" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="114"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
-      <c r="F5" s="112"/>
-      <c r="G5" s="112"/>
-      <c r="H5" s="112"/>
-      <c r="I5" s="113"/>
+      <c r="C5" s="129"/>
+      <c r="D5" s="130"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="130"/>
+      <c r="G5" s="130"/>
+      <c r="H5" s="130"/>
+      <c r="I5" s="131"/>
       <c r="J5" s="21"/>
     </row>
     <row r="6" spans="1:78" x14ac:dyDescent="0.55000000000000004">
@@ -34184,13 +34178,13 @@
       <c r="B6" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C6" s="114"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="112"/>
-      <c r="F6" s="112"/>
-      <c r="G6" s="112"/>
-      <c r="H6" s="112"/>
-      <c r="I6" s="113"/>
+      <c r="C6" s="129"/>
+      <c r="D6" s="130"/>
+      <c r="E6" s="130"/>
+      <c r="F6" s="130"/>
+      <c r="G6" s="130"/>
+      <c r="H6" s="130"/>
+      <c r="I6" s="131"/>
       <c r="J6" s="21"/>
     </row>
     <row r="7" spans="1:78" x14ac:dyDescent="0.55000000000000004">
@@ -34198,13 +34192,13 @@
       <c r="B7" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="114"/>
-      <c r="D7" s="112"/>
-      <c r="E7" s="112"/>
-      <c r="F7" s="112"/>
-      <c r="G7" s="112"/>
-      <c r="H7" s="112"/>
-      <c r="I7" s="113"/>
+      <c r="C7" s="129"/>
+      <c r="D7" s="130"/>
+      <c r="E7" s="130"/>
+      <c r="F7" s="130"/>
+      <c r="G7" s="130"/>
+      <c r="H7" s="130"/>
+      <c r="I7" s="131"/>
       <c r="J7" s="21"/>
     </row>
     <row r="8" spans="1:78" x14ac:dyDescent="0.55000000000000004">
@@ -34212,13 +34206,13 @@
       <c r="B8" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C8" s="114"/>
-      <c r="D8" s="112"/>
-      <c r="E8" s="112"/>
-      <c r="F8" s="112"/>
-      <c r="G8" s="112"/>
-      <c r="H8" s="112"/>
-      <c r="I8" s="113"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="130"/>
+      <c r="E8" s="130"/>
+      <c r="F8" s="130"/>
+      <c r="G8" s="130"/>
+      <c r="H8" s="130"/>
+      <c r="I8" s="131"/>
       <c r="J8" s="21"/>
     </row>
     <row r="9" spans="1:78" x14ac:dyDescent="0.55000000000000004">
@@ -34226,13 +34220,13 @@
       <c r="B9" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="C9" s="115"/>
-      <c r="D9" s="116"/>
-      <c r="E9" s="116"/>
-      <c r="F9" s="116"/>
-      <c r="G9" s="116"/>
-      <c r="H9" s="116"/>
-      <c r="I9" s="117"/>
+      <c r="C9" s="148"/>
+      <c r="D9" s="149"/>
+      <c r="E9" s="149"/>
+      <c r="F9" s="149"/>
+      <c r="G9" s="149"/>
+      <c r="H9" s="149"/>
+      <c r="I9" s="150"/>
       <c r="J9" s="21"/>
     </row>
     <row r="10" spans="1:78" x14ac:dyDescent="0.55000000000000004">
@@ -34240,13 +34234,13 @@
       <c r="B10" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C10" s="114"/>
-      <c r="D10" s="112"/>
-      <c r="E10" s="112"/>
-      <c r="F10" s="112"/>
-      <c r="G10" s="112"/>
-      <c r="H10" s="112"/>
-      <c r="I10" s="113"/>
+      <c r="C10" s="129"/>
+      <c r="D10" s="130"/>
+      <c r="E10" s="130"/>
+      <c r="F10" s="130"/>
+      <c r="G10" s="130"/>
+      <c r="H10" s="130"/>
+      <c r="I10" s="131"/>
       <c r="J10" s="21"/>
     </row>
     <row r="11" spans="1:78" x14ac:dyDescent="0.55000000000000004">
@@ -34254,13 +34248,13 @@
       <c r="B11" s="9" t="s">
         <v>345</v>
       </c>
-      <c r="C11" s="114"/>
-      <c r="D11" s="112"/>
-      <c r="E11" s="112"/>
-      <c r="F11" s="112"/>
-      <c r="G11" s="112"/>
-      <c r="H11" s="112"/>
-      <c r="I11" s="113"/>
+      <c r="C11" s="129"/>
+      <c r="D11" s="130"/>
+      <c r="E11" s="130"/>
+      <c r="F11" s="130"/>
+      <c r="G11" s="130"/>
+      <c r="H11" s="130"/>
+      <c r="I11" s="131"/>
       <c r="J11" s="21"/>
     </row>
     <row r="12" spans="1:78" x14ac:dyDescent="0.55000000000000004">
@@ -34268,13 +34262,13 @@
       <c r="B12" s="9" t="s">
         <v>346</v>
       </c>
-      <c r="C12" s="114"/>
-      <c r="D12" s="112"/>
-      <c r="E12" s="112"/>
-      <c r="F12" s="112"/>
-      <c r="G12" s="112"/>
-      <c r="H12" s="112"/>
-      <c r="I12" s="113"/>
+      <c r="C12" s="129"/>
+      <c r="D12" s="130"/>
+      <c r="E12" s="130"/>
+      <c r="F12" s="130"/>
+      <c r="G12" s="130"/>
+      <c r="H12" s="130"/>
+      <c r="I12" s="131"/>
       <c r="J12" s="21"/>
     </row>
     <row r="13" spans="1:78" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -34282,66 +34276,66 @@
       <c r="B13" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="111"/>
-      <c r="D13" s="112"/>
-      <c r="E13" s="112"/>
-      <c r="F13" s="112"/>
-      <c r="G13" s="112"/>
-      <c r="H13" s="112"/>
-      <c r="I13" s="113"/>
+      <c r="C13" s="124"/>
+      <c r="D13" s="130"/>
+      <c r="E13" s="130"/>
+      <c r="F13" s="130"/>
+      <c r="G13" s="130"/>
+      <c r="H13" s="130"/>
+      <c r="I13" s="131"/>
       <c r="J13" s="21"/>
     </row>
     <row r="14" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="20"/>
-      <c r="B14" s="135" t="s">
+      <c r="B14" s="110" t="s">
         <v>117</v>
       </c>
-      <c r="C14" s="154" t="s">
+      <c r="C14" s="113" t="s">
         <v>337</v>
       </c>
-      <c r="D14" s="155"/>
-      <c r="E14" s="124"/>
-      <c r="F14" s="125"/>
-      <c r="G14" s="125"/>
-      <c r="H14" s="125"/>
-      <c r="I14" s="126"/>
+      <c r="D14" s="114"/>
+      <c r="E14" s="132"/>
+      <c r="F14" s="133"/>
+      <c r="G14" s="133"/>
+      <c r="H14" s="133"/>
+      <c r="I14" s="134"/>
       <c r="J14" s="21"/>
     </row>
     <row r="15" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="20"/>
-      <c r="B15" s="136"/>
-      <c r="C15" s="114" t="s">
+      <c r="B15" s="111"/>
+      <c r="C15" s="129" t="s">
         <v>338</v>
       </c>
-      <c r="D15" s="138"/>
-      <c r="E15" s="114"/>
-      <c r="F15" s="112"/>
-      <c r="G15" s="112"/>
-      <c r="H15" s="112"/>
-      <c r="I15" s="113"/>
+      <c r="D15" s="141"/>
+      <c r="E15" s="129"/>
+      <c r="F15" s="130"/>
+      <c r="G15" s="130"/>
+      <c r="H15" s="130"/>
+      <c r="I15" s="131"/>
       <c r="J15" s="21"/>
     </row>
     <row r="16" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="20"/>
-      <c r="B16" s="136"/>
-      <c r="C16" s="111" t="s">
+      <c r="B16" s="111"/>
+      <c r="C16" s="124" t="s">
         <v>339</v>
       </c>
-      <c r="D16" s="139"/>
-      <c r="E16" s="114"/>
-      <c r="F16" s="133"/>
-      <c r="G16" s="133"/>
-      <c r="H16" s="133"/>
-      <c r="I16" s="140"/>
+      <c r="D16" s="125"/>
+      <c r="E16" s="129"/>
+      <c r="F16" s="120"/>
+      <c r="G16" s="120"/>
+      <c r="H16" s="120"/>
+      <c r="I16" s="142"/>
       <c r="J16" s="21"/>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="20"/>
-      <c r="B17" s="136"/>
-      <c r="C17" s="111" t="s">
+      <c r="B17" s="111"/>
+      <c r="C17" s="124" t="s">
         <v>340</v>
       </c>
-      <c r="D17" s="139"/>
+      <c r="D17" s="125"/>
       <c r="E17" s="64"/>
       <c r="F17" s="65"/>
       <c r="G17" s="65"/>
@@ -34351,74 +34345,74 @@
     </row>
     <row r="18" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A18" s="20"/>
-      <c r="B18" s="153"/>
-      <c r="C18" s="141" t="s">
+      <c r="B18" s="112"/>
+      <c r="C18" s="143" t="s">
         <v>336</v>
       </c>
-      <c r="D18" s="142"/>
-      <c r="E18" s="141"/>
-      <c r="F18" s="143"/>
-      <c r="G18" s="143"/>
-      <c r="H18" s="143"/>
-      <c r="I18" s="144"/>
+      <c r="D18" s="144"/>
+      <c r="E18" s="143"/>
+      <c r="F18" s="145"/>
+      <c r="G18" s="145"/>
+      <c r="H18" s="145"/>
+      <c r="I18" s="146"/>
       <c r="J18" s="21"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="20"/>
-      <c r="B19" s="135" t="s">
+      <c r="B19" s="110" t="s">
         <v>118</v>
       </c>
       <c r="C19" s="12">
         <v>1</v>
       </c>
-      <c r="D19" s="137"/>
-      <c r="E19" s="125"/>
-      <c r="F19" s="125"/>
-      <c r="G19" s="125"/>
-      <c r="H19" s="125"/>
-      <c r="I19" s="126"/>
+      <c r="D19" s="140"/>
+      <c r="E19" s="133"/>
+      <c r="F19" s="133"/>
+      <c r="G19" s="133"/>
+      <c r="H19" s="133"/>
+      <c r="I19" s="134"/>
       <c r="J19" s="21"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="20"/>
-      <c r="B20" s="136"/>
+      <c r="B20" s="111"/>
       <c r="C20" s="13">
         <v>2</v>
       </c>
-      <c r="D20" s="114"/>
-      <c r="E20" s="112"/>
-      <c r="F20" s="112"/>
-      <c r="G20" s="112"/>
-      <c r="H20" s="112"/>
-      <c r="I20" s="113"/>
+      <c r="D20" s="129"/>
+      <c r="E20" s="130"/>
+      <c r="F20" s="130"/>
+      <c r="G20" s="130"/>
+      <c r="H20" s="130"/>
+      <c r="I20" s="131"/>
       <c r="J20" s="21"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="20"/>
-      <c r="B21" s="136"/>
+      <c r="B21" s="111"/>
       <c r="C21" s="13">
         <v>3</v>
       </c>
-      <c r="D21" s="114"/>
-      <c r="E21" s="112"/>
-      <c r="F21" s="112"/>
-      <c r="G21" s="112"/>
-      <c r="H21" s="112"/>
-      <c r="I21" s="113"/>
+      <c r="D21" s="129"/>
+      <c r="E21" s="130"/>
+      <c r="F21" s="130"/>
+      <c r="G21" s="130"/>
+      <c r="H21" s="130"/>
+      <c r="I21" s="131"/>
       <c r="J21" s="21"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="20"/>
-      <c r="B22" s="136"/>
+      <c r="B22" s="111"/>
       <c r="C22" s="13">
         <v>4</v>
       </c>
-      <c r="D22" s="114"/>
-      <c r="E22" s="112"/>
-      <c r="F22" s="112"/>
-      <c r="G22" s="112"/>
-      <c r="H22" s="112"/>
-      <c r="I22" s="113"/>
+      <c r="D22" s="129"/>
+      <c r="E22" s="130"/>
+      <c r="F22" s="130"/>
+      <c r="G22" s="130"/>
+      <c r="H22" s="130"/>
+      <c r="I22" s="131"/>
       <c r="J22" s="21"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -34427,12 +34421,12 @@
       <c r="C23" s="13">
         <v>5</v>
       </c>
-      <c r="D23" s="114"/>
-      <c r="E23" s="112"/>
-      <c r="F23" s="112"/>
-      <c r="G23" s="112"/>
-      <c r="H23" s="112"/>
-      <c r="I23" s="113"/>
+      <c r="D23" s="129"/>
+      <c r="E23" s="130"/>
+      <c r="F23" s="130"/>
+      <c r="G23" s="130"/>
+      <c r="H23" s="130"/>
+      <c r="I23" s="131"/>
       <c r="J23" s="21"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -34441,12 +34435,12 @@
       <c r="C24" s="13">
         <v>6</v>
       </c>
-      <c r="D24" s="114"/>
-      <c r="E24" s="112"/>
-      <c r="F24" s="112"/>
-      <c r="G24" s="112"/>
-      <c r="H24" s="112"/>
-      <c r="I24" s="113"/>
+      <c r="D24" s="129"/>
+      <c r="E24" s="130"/>
+      <c r="F24" s="130"/>
+      <c r="G24" s="130"/>
+      <c r="H24" s="130"/>
+      <c r="I24" s="131"/>
       <c r="J24" s="21"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -34455,12 +34449,12 @@
       <c r="C25" s="13">
         <v>7</v>
       </c>
-      <c r="D25" s="114"/>
-      <c r="E25" s="112"/>
-      <c r="F25" s="112"/>
-      <c r="G25" s="112"/>
-      <c r="H25" s="112"/>
-      <c r="I25" s="113"/>
+      <c r="D25" s="129"/>
+      <c r="E25" s="130"/>
+      <c r="F25" s="130"/>
+      <c r="G25" s="130"/>
+      <c r="H25" s="130"/>
+      <c r="I25" s="131"/>
       <c r="J25" s="21"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -34469,12 +34463,12 @@
       <c r="C26" s="13">
         <v>8</v>
       </c>
-      <c r="D26" s="114"/>
-      <c r="E26" s="112"/>
-      <c r="F26" s="112"/>
-      <c r="G26" s="112"/>
-      <c r="H26" s="112"/>
-      <c r="I26" s="113"/>
+      <c r="D26" s="129"/>
+      <c r="E26" s="130"/>
+      <c r="F26" s="130"/>
+      <c r="G26" s="130"/>
+      <c r="H26" s="130"/>
+      <c r="I26" s="131"/>
       <c r="J26" s="21"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -34483,12 +34477,12 @@
       <c r="C27" s="13">
         <v>9</v>
       </c>
-      <c r="D27" s="114"/>
-      <c r="E27" s="112"/>
-      <c r="F27" s="112"/>
-      <c r="G27" s="112"/>
-      <c r="H27" s="112"/>
-      <c r="I27" s="113"/>
+      <c r="D27" s="129"/>
+      <c r="E27" s="130"/>
+      <c r="F27" s="130"/>
+      <c r="G27" s="130"/>
+      <c r="H27" s="130"/>
+      <c r="I27" s="131"/>
       <c r="J27" s="21"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -34497,12 +34491,12 @@
       <c r="C28" s="13">
         <v>10</v>
       </c>
-      <c r="D28" s="114"/>
-      <c r="E28" s="112"/>
-      <c r="F28" s="112"/>
-      <c r="G28" s="112"/>
-      <c r="H28" s="112"/>
-      <c r="I28" s="113"/>
+      <c r="D28" s="129"/>
+      <c r="E28" s="130"/>
+      <c r="F28" s="130"/>
+      <c r="G28" s="130"/>
+      <c r="H28" s="130"/>
+      <c r="I28" s="131"/>
       <c r="J28" s="21"/>
     </row>
     <row r="29" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -34511,151 +34505,151 @@
       <c r="C29" s="13" t="s">
         <v>336</v>
       </c>
-      <c r="D29" s="114"/>
-      <c r="E29" s="112"/>
-      <c r="F29" s="112"/>
-      <c r="G29" s="112"/>
-      <c r="H29" s="112"/>
-      <c r="I29" s="113"/>
+      <c r="D29" s="129"/>
+      <c r="E29" s="130"/>
+      <c r="F29" s="130"/>
+      <c r="G29" s="130"/>
+      <c r="H29" s="130"/>
+      <c r="I29" s="131"/>
       <c r="J29" s="21"/>
     </row>
     <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="20"/>
-      <c r="B30" s="127" t="s">
+      <c r="B30" s="135" t="s">
         <v>196</v>
       </c>
-      <c r="C30" s="129"/>
-      <c r="D30" s="130"/>
-      <c r="E30" s="131"/>
-      <c r="F30" s="147" t="s">
+      <c r="C30" s="137"/>
+      <c r="D30" s="138"/>
+      <c r="E30" s="139"/>
+      <c r="F30" s="126" t="s">
         <v>343</v>
       </c>
-      <c r="G30" s="148"/>
-      <c r="H30" s="149"/>
+      <c r="G30" s="127"/>
+      <c r="H30" s="128"/>
       <c r="I30" s="14"/>
       <c r="J30" s="21"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="20"/>
-      <c r="B31" s="128"/>
-      <c r="C31" s="132" t="s">
+      <c r="B31" s="136"/>
+      <c r="C31" s="119" t="s">
         <v>197</v>
       </c>
-      <c r="D31" s="133"/>
-      <c r="E31" s="134"/>
-      <c r="F31" s="150"/>
-      <c r="G31" s="151"/>
-      <c r="H31" s="152"/>
+      <c r="D31" s="120"/>
+      <c r="E31" s="121"/>
+      <c r="F31" s="116"/>
+      <c r="G31" s="117"/>
+      <c r="H31" s="118"/>
       <c r="I31" s="15"/>
       <c r="J31" s="21"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="20"/>
-      <c r="B32" s="128"/>
-      <c r="C32" s="132" t="s">
+      <c r="B32" s="136"/>
+      <c r="C32" s="119" t="s">
         <v>198</v>
       </c>
-      <c r="D32" s="133"/>
-      <c r="E32" s="134"/>
-      <c r="F32" s="150"/>
-      <c r="G32" s="151"/>
-      <c r="H32" s="152"/>
+      <c r="D32" s="120"/>
+      <c r="E32" s="121"/>
+      <c r="F32" s="116"/>
+      <c r="G32" s="117"/>
+      <c r="H32" s="118"/>
       <c r="I32" s="15"/>
       <c r="J32" s="21"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="20"/>
-      <c r="B33" s="128"/>
-      <c r="C33" s="132" t="s">
+      <c r="B33" s="136"/>
+      <c r="C33" s="119" t="s">
         <v>342</v>
       </c>
-      <c r="D33" s="133"/>
-      <c r="E33" s="134"/>
-      <c r="F33" s="150" t="s">
+      <c r="D33" s="120"/>
+      <c r="E33" s="121"/>
+      <c r="F33" s="116" t="s">
         <v>199</v>
       </c>
-      <c r="G33" s="151"/>
-      <c r="H33" s="152"/>
+      <c r="G33" s="117"/>
+      <c r="H33" s="118"/>
       <c r="I33" s="15"/>
       <c r="J33" s="21"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="20"/>
-      <c r="B34" s="128"/>
-      <c r="C34" s="132" t="s">
+      <c r="B34" s="136"/>
+      <c r="C34" s="119" t="s">
         <v>240</v>
       </c>
-      <c r="D34" s="133"/>
-      <c r="E34" s="134"/>
-      <c r="F34" s="150" t="s">
+      <c r="D34" s="120"/>
+      <c r="E34" s="121"/>
+      <c r="F34" s="116" t="s">
         <v>199</v>
       </c>
-      <c r="G34" s="151"/>
-      <c r="H34" s="152"/>
+      <c r="G34" s="117"/>
+      <c r="H34" s="118"/>
       <c r="I34" s="15"/>
       <c r="J34" s="21"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="20"/>
-      <c r="B35" s="128"/>
-      <c r="C35" s="132" t="s">
+      <c r="B35" s="136"/>
+      <c r="C35" s="119" t="s">
         <v>241</v>
       </c>
-      <c r="D35" s="133"/>
-      <c r="E35" s="134"/>
-      <c r="F35" s="150" t="s">
+      <c r="D35" s="120"/>
+      <c r="E35" s="121"/>
+      <c r="F35" s="116" t="s">
         <v>199</v>
       </c>
-      <c r="G35" s="151"/>
-      <c r="H35" s="152"/>
+      <c r="G35" s="117"/>
+      <c r="H35" s="118"/>
       <c r="I35" s="15"/>
       <c r="J35" s="21"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="20"/>
-      <c r="B36" s="128"/>
-      <c r="C36" s="132" t="s">
+      <c r="B36" s="136"/>
+      <c r="C36" s="119" t="s">
         <v>341</v>
       </c>
-      <c r="D36" s="133"/>
-      <c r="E36" s="134"/>
-      <c r="F36" s="150" t="s">
+      <c r="D36" s="120"/>
+      <c r="E36" s="121"/>
+      <c r="F36" s="116" t="s">
         <v>199</v>
       </c>
-      <c r="G36" s="151"/>
-      <c r="H36" s="152"/>
+      <c r="G36" s="117"/>
+      <c r="H36" s="118"/>
       <c r="I36" s="15"/>
       <c r="J36" s="21"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="20"/>
-      <c r="B37" s="128"/>
-      <c r="C37" s="132" t="s">
+      <c r="B37" s="136"/>
+      <c r="C37" s="119" t="s">
         <v>242</v>
       </c>
-      <c r="D37" s="133"/>
-      <c r="E37" s="134"/>
-      <c r="F37" s="150" t="s">
+      <c r="D37" s="120"/>
+      <c r="E37" s="121"/>
+      <c r="F37" s="116" t="s">
         <v>199</v>
       </c>
-      <c r="G37" s="151"/>
-      <c r="H37" s="152"/>
+      <c r="G37" s="117"/>
+      <c r="H37" s="118"/>
       <c r="I37" s="15"/>
       <c r="J37" s="21"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="20"/>
-      <c r="B38" s="128"/>
-      <c r="C38" s="132" t="s">
+      <c r="B38" s="136"/>
+      <c r="C38" s="119" t="s">
         <v>243</v>
       </c>
-      <c r="D38" s="133"/>
-      <c r="E38" s="134"/>
-      <c r="F38" s="150" t="s">
+      <c r="D38" s="120"/>
+      <c r="E38" s="121"/>
+      <c r="F38" s="116" t="s">
         <v>199</v>
       </c>
-      <c r="G38" s="151"/>
-      <c r="H38" s="152"/>
+      <c r="G38" s="117"/>
+      <c r="H38" s="118"/>
       <c r="I38" s="15"/>
       <c r="J38" s="21"/>
     </row>
@@ -34664,20 +34658,20 @@
       <c r="B39" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="C39" s="145"/>
-      <c r="D39" s="145"/>
-      <c r="E39" s="145"/>
-      <c r="F39" s="145"/>
-      <c r="G39" s="145"/>
-      <c r="H39" s="145"/>
-      <c r="I39" s="146"/>
+      <c r="C39" s="122"/>
+      <c r="D39" s="122"/>
+      <c r="E39" s="122"/>
+      <c r="F39" s="122"/>
+      <c r="G39" s="122"/>
+      <c r="H39" s="122"/>
+      <c r="I39" s="123"/>
       <c r="J39" s="21"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="20"/>
       <c r="B40" s="22"/>
-      <c r="C40" s="156"/>
-      <c r="D40" s="156"/>
+      <c r="C40" s="115"/>
+      <c r="D40" s="115"/>
       <c r="E40" s="22"/>
       <c r="F40" s="22"/>
       <c r="G40" s="22"/>
@@ -34699,6 +34693,44 @@
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="C10:I10"/>
+    <mergeCell ref="C11:I11"/>
+    <mergeCell ref="C12:I12"/>
+    <mergeCell ref="B3:I4"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="E14:I14"/>
+    <mergeCell ref="B30:B38"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="D19:I19"/>
+    <mergeCell ref="D20:I20"/>
+    <mergeCell ref="D21:I21"/>
+    <mergeCell ref="D22:I22"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:I15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="C39:I39"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="D23:I23"/>
+    <mergeCell ref="D24:I24"/>
+    <mergeCell ref="D25:I25"/>
+    <mergeCell ref="D26:I26"/>
+    <mergeCell ref="D27:I27"/>
+    <mergeCell ref="D28:I28"/>
+    <mergeCell ref="D29:I29"/>
+    <mergeCell ref="F36:H36"/>
     <mergeCell ref="B14:B18"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C40:D40"/>
@@ -34715,44 +34747,6 @@
     <mergeCell ref="C38:E38"/>
     <mergeCell ref="C36:E36"/>
     <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C39:I39"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="D23:I23"/>
-    <mergeCell ref="D24:I24"/>
-    <mergeCell ref="D25:I25"/>
-    <mergeCell ref="D26:I26"/>
-    <mergeCell ref="D27:I27"/>
-    <mergeCell ref="D28:I28"/>
-    <mergeCell ref="D29:I29"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="E14:I14"/>
-    <mergeCell ref="B30:B38"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="D19:I19"/>
-    <mergeCell ref="D20:I20"/>
-    <mergeCell ref="D21:I21"/>
-    <mergeCell ref="D22:I22"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:I15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="C8:I8"/>
-    <mergeCell ref="C9:I9"/>
-    <mergeCell ref="C10:I10"/>
-    <mergeCell ref="C11:I11"/>
-    <mergeCell ref="C12:I12"/>
-    <mergeCell ref="B3:I4"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="C7:I7"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -34764,7 +34758,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EF082ED-214B-4421-A448-CD98E7D28979}">
   <dimension ref="A1:BY26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
@@ -35023,6 +35017,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D47EB396FE081D4485E46F2BB5A816BE" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9f025edd3bb6c145477cc0751d3041a3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="617a1b0e-0b35-49af-848d-aa0d88eb4391" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1fa5b47e14240031dc6cd3d61c8b3603" ns3:_="">
     <xsd:import namespace="617a1b0e-0b35-49af-848d-aa0d88eb4391"/>
@@ -35148,12 +35148,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -35164,6 +35158,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A58519DC-97D4-44C8-8C02-B225F4453FDF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="617a1b0e-0b35-49af-848d-aa0d88eb4391"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6CDE9DB-F3BF-44E1-8765-D39599633ECF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -35181,22 +35191,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A58519DC-97D4-44C8-8C02-B225F4453FDF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="617a1b0e-0b35-49af-848d-aa0d88eb4391"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9AD77191-1161-4B2C-A11F-7E842B6F88C0}">
   <ds:schemaRefs>

</xml_diff>